<commit_message>
TestNG And Advanced Actions
</commit_message>
<xml_diff>
--- a/Test_Data/doc1.xlsx
+++ b/Test_Data/doc1.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aynigar\CubeCartApplication2021\Test_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abdullah\IdeaProjects\cubecartapplication2021.11\Test_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D9632C5-4425-425F-A48B-00A25ABA088F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login-Info" sheetId="1" r:id="rId1"/>
-    <sheet name="Product_Info" sheetId="2" r:id="rId2"/>
+    <sheet name="Product_Info2" sheetId="3" r:id="rId2"/>
+    <sheet name="Product_Info" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t>Password</t>
   </si>
@@ -81,7 +83,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -392,20 +394,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.81640625" customWidth="1"/>
-    <col min="2" max="2" width="18.54296875" customWidth="1"/>
+    <col min="1" max="1" width="21.77734375" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -413,7 +415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -421,7 +423,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -435,22 +437,98 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF74587E-675E-4555-93DA-90FAB590219C}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.77734375" customWidth="1"/>
+    <col min="2" max="2" width="22.21875" customWidth="1"/>
+    <col min="3" max="3" width="26.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B1" sqref="B1:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.26953125" customWidth="1"/>
+    <col min="1" max="1" width="18.21875" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="17.90625" customWidth="1"/>
-    <col min="4" max="4" width="15.453125" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -464,7 +542,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -478,7 +556,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -492,7 +570,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>

</xml_diff>